<commit_message>
[Welder] More work in the topic.
</commit_message>
<xml_diff>
--- a/inverter-welder/concepts/08_magnum_power_vip_4000/improvements/02/sch/potentiometers.xlsx
+++ b/inverter-welder/concepts/08_magnum_power_vip_4000/improvements/02/sch/potentiometers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\prj\dev-test\sources\various\sandbox\inverter-welder\concepts\08_magnum_power_vip_4000\improvements\02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\prj\dev-test\sources\various\sandbox\inverter-welder\concepts\08_magnum_power_vip_4000\improvements\02\sch\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -56,13 +56,13 @@
     <t>P2</t>
   </si>
   <si>
-    <t>VR3</t>
-  </si>
-  <si>
     <t>do masy</t>
   </si>
   <si>
     <t>do VCC</t>
+  </si>
+  <si>
+    <t>VR2</t>
   </si>
 </sst>
 </file>
@@ -387,9 +387,9 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -400,7 +400,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -411,7 +411,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -422,7 +422,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -433,59 +433,59 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
       </c>
       <c r="D9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
       <c r="B10">
-        <v>17.5</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
       <c r="B12">
         <f>$B$5/($B$9 + $B$2 + $B$10)</f>
-        <v>8.9014084507042263E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9.4047619047619047E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>0</v>
       </c>
       <c r="B13">
         <f>$B$10 * $B$12</f>
-        <v>1.5577464788732396</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.5047619047619047</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>1</v>
       </c>
       <c r="B14">
         <f>($B$2+$B$10)*$B$12</f>
-        <v>6.0084507042253525</v>
+        <v>6.2071428571428573</v>
       </c>
     </row>
   </sheetData>

</xml_diff>